<commit_message>
Update excel with 4b
</commit_message>
<xml_diff>
--- a/02_assignment/02_assignment_02_03.xlsx
+++ b/02_assignment/02_assignment_02_03.xlsx
@@ -8,60 +8,74 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumente\UvA\03_SSO_Statics_Simulation_Optimization\2022_sso_group4\02_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B15006-F882-4326-97FF-C85319AD2F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428D2530-178F-4C11-A97A-945DE42D926F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32670" yWindow="2010" windowWidth="23175" windowHeight="11835" activeTab="3" xr2:uid="{FA1A1E67-CE5E-0248-89A6-9923701A5D4A}"/>
+    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4" xr2:uid="{FA1A1E67-CE5E-0248-89A6-9923701A5D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="03_a" sheetId="1" r:id="rId1"/>
     <sheet name="03_b" sheetId="4" r:id="rId2"/>
     <sheet name="03_c" sheetId="3" r:id="rId3"/>
     <sheet name="04_a" sheetId="5" r:id="rId4"/>
+    <sheet name="04_b" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'03_a'!$B$3:$B$7</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'03_b'!$B$3:$B$8</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'03_c'!$B$3:$B$7</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'04_a'!$B$11:$E$13</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'04_b'!$B$11:$E$13</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'03_a'!$B$11</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'03_b'!$B$11</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'03_c'!$B$11</definedName>
     <definedName name="solver_lhs1" localSheetId="3" hidden="1">'04_a'!$B$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'04_b'!$B$14</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'03_a'!$B$12</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'03_b'!$B$12</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'03_c'!$B$12</definedName>
     <definedName name="solver_lhs2" localSheetId="3" hidden="1">'04_a'!$C$14</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'04_b'!$C$14</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'03_a'!$B$13</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">'03_b'!$B$13</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'03_c'!$B$13</definedName>
     <definedName name="solver_lhs3" localSheetId="3" hidden="1">'04_a'!$D$14</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">'04_b'!$D$14</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'03_a'!$B$14</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">'03_b'!$B$14</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">'03_c'!$B$14</definedName>
     <definedName name="solver_lhs4" localSheetId="3" hidden="1">'04_a'!$E$14</definedName>
+    <definedName name="solver_lhs4" localSheetId="4" hidden="1">'04_b'!$E$14</definedName>
     <definedName name="solver_lhs5" localSheetId="1" hidden="1">'03_b'!$B$7</definedName>
     <definedName name="solver_lhs5" localSheetId="2" hidden="1">'03_c'!$B$3:$B$7</definedName>
     <definedName name="solver_lhs5" localSheetId="3" hidden="1">'04_a'!$F$11</definedName>
+    <definedName name="solver_lhs5" localSheetId="4" hidden="1">'04_b'!$F$11</definedName>
     <definedName name="solver_lhs6" localSheetId="3" hidden="1">'04_a'!$F$12</definedName>
+    <definedName name="solver_lhs6" localSheetId="4" hidden="1">'04_b'!$F$12</definedName>
     <definedName name="solver_lhs7" localSheetId="3" hidden="1">'04_a'!$F$13</definedName>
+    <definedName name="solver_lhs7" localSheetId="4" hidden="1">'04_b'!$F$13</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="2" hidden="1">1</definedName>
@@ -69,126 +83,161 @@
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">7</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">7</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'03_a'!$A$19</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'03_b'!$A$19</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'03_c'!$A$19</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">'04_a'!$A$17</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'04_b'!$A$17</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_rel5" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">'03_a'!$D$11</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'03_b'!$D$11</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">'03_c'!$D$11</definedName>
     <definedName name="solver_rhs1" localSheetId="3" hidden="1">'04_a'!$B$8</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">'04_b'!$B$8</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'03_a'!$D$12</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">'03_b'!$D$12</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">'03_c'!$D$12</definedName>
     <definedName name="solver_rhs2" localSheetId="3" hidden="1">'04_a'!$C$8</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">'04_b'!$C$8</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'03_a'!$D$13</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">'03_b'!$D$13</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">'03_c'!$D$13</definedName>
     <definedName name="solver_rhs3" localSheetId="3" hidden="1">'04_a'!$D$8</definedName>
+    <definedName name="solver_rhs3" localSheetId="4" hidden="1">'04_b'!$D$8</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">'03_a'!$D$14</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">'03_b'!$D$14</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">'03_c'!$D$14</definedName>
     <definedName name="solver_rhs4" localSheetId="3" hidden="1">'04_a'!$E$8</definedName>
+    <definedName name="solver_rhs4" localSheetId="4" hidden="1">'04_b'!$E$8</definedName>
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">'03_b'!$D$15</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">"integer"</definedName>
     <definedName name="solver_rhs5" localSheetId="3" hidden="1">'04_a'!$F$5</definedName>
+    <definedName name="solver_rhs5" localSheetId="4" hidden="1">'04_b'!$F$5</definedName>
     <definedName name="solver_rhs6" localSheetId="3" hidden="1">'04_a'!$F$6</definedName>
+    <definedName name="solver_rhs6" localSheetId="4" hidden="1">'04_b'!$F$6</definedName>
     <definedName name="solver_rhs7" localSheetId="3" hidden="1">'04_a'!$F$7</definedName>
+    <definedName name="solver_rhs7" localSheetId="4" hidden="1">'04_b'!$F$7</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -210,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
   <si>
     <t>Carrots</t>
   </si>
@@ -282,15 +331,37 @@
   </si>
   <si>
     <t>Sums</t>
+  </si>
+  <si>
+    <t>Inflow</t>
+  </si>
+  <si>
+    <t>Decision y_ij</t>
+  </si>
+  <si>
+    <t>Fixed Cost</t>
+  </si>
+  <si>
+    <t>Total Fixed Costs</t>
+  </si>
+  <si>
+    <t>Objective Fixed Costs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -310,8 +381,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +430,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -364,17 +448,22 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1497,7 +1586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5276B8C9-8A84-44D6-9588-524B8B466C18}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -1725,4 +1814,340 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB1C8C8-2960-4D74-B02D-5741ABED90CB}">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="8" max="8" width="14.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>20</v>
+      </c>
+      <c r="E5" s="9">
+        <v>11</v>
+      </c>
+      <c r="F5" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9">
+        <v>12</v>
+      </c>
+      <c r="C6" s="9">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9">
+        <v>20</v>
+      </c>
+      <c r="F6" s="11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
+        <v>14</v>
+      </c>
+      <c r="D7" s="9">
+        <v>16</v>
+      </c>
+      <c r="E7" s="9">
+        <v>18</v>
+      </c>
+      <c r="F7" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="11">
+        <v>10</v>
+      </c>
+      <c r="C8" s="11">
+        <v>15</v>
+      </c>
+      <c r="D8" s="11">
+        <v>15</v>
+      </c>
+      <c r="E8" s="11">
+        <v>20</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>15</v>
+      </c>
+      <c r="F11" s="6">
+        <f xml:space="preserve"> SUM(B11:E11)</f>
+        <v>20</v>
+      </c>
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <f xml:space="preserve"> IF(B11 &gt;0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" ref="J11:L13" si="0" xml:space="preserve"> IF(C11 &gt;0, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8">
+        <v>15</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <f xml:space="preserve"> SUM(B12:E12)</f>
+        <v>25</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" ref="I12:I13" si="1" xml:space="preserve"> IF(B12 &gt;0, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="8">
+        <v>10</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="F13" s="6">
+        <f xml:space="preserve"> SUM(B13:E13)</f>
+        <v>15</v>
+      </c>
+      <c r="H13" s="7">
+        <v>3</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6">
+        <f xml:space="preserve"> SUM(B11:B13)</f>
+        <v>10</v>
+      </c>
+      <c r="C14" s="6">
+        <f xml:space="preserve"> SUM(C11:C13)</f>
+        <v>15</v>
+      </c>
+      <c r="D14" s="6">
+        <f xml:space="preserve"> SUM(D11:D13)</f>
+        <v>15</v>
+      </c>
+      <c r="E14" s="6">
+        <f xml:space="preserve"> SUM(E11:E13)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <f>SUMPRODUCT(B5:E7, B11:E13)</f>
+        <v>460</v>
+      </c>
+      <c r="B17" s="5">
+        <f xml:space="preserve"> A17 + I17</f>
+        <v>1060</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="4">
+        <f xml:space="preserve"> SUM(I11:L13)*100</f>
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add more math for 2.3.b and c
</commit_message>
<xml_diff>
--- a/02_assignment/02_assignment_02_03.xlsx
+++ b/02_assignment/02_assignment_02_03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumente\UvA\03_SSO_Statics_Simulation_Optimization\2022_sso_group4\02_assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katringrunert/Projects/Uni/sso/exercises/02_assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428D2530-178F-4C11-A97A-945DE42D926F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E2CC35-32D4-A845-9516-601658CA11FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4" xr2:uid="{FA1A1E67-CE5E-0248-89A6-9923701A5D4A}"/>
+    <workbookView xWindow="15420" yWindow="520" windowWidth="20420" windowHeight="20280" activeTab="1" xr2:uid="{FA1A1E67-CE5E-0248-89A6-9923701A5D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="03_a" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="solver_adj" localSheetId="1" hidden="1">'03_b'!$B$3:$B$8</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'03_c'!$B$3:$B$7</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'04_a'!$B$11:$E$13</definedName>
-    <definedName name="solver_adj" localSheetId="4" hidden="1">'04_b'!$B$11:$E$13</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'04_b'!$B$11:$E$13,'04_b'!$I$11:$L$13</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
@@ -51,34 +51,39 @@
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'03_a'!$B$11</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'03_b'!$B$11</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'03_c'!$B$11</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'04_a'!$B$14</definedName>
-    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'04_b'!$B$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'04_a'!$B$11:$E$13</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'04_b'!$B$11:$E$13</definedName>
+    <definedName name="solver_lhs10" localSheetId="4" hidden="1">'04_b'!$I$11:$L$13</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'03_a'!$B$12</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'03_b'!$B$12</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'03_c'!$B$12</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'04_a'!$C$14</definedName>
-    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'04_b'!$C$14</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'04_a'!$B$14:$E$14</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'04_b'!$B$14:$E$14</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'03_a'!$B$13</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">'03_b'!$B$13</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'03_c'!$B$13</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'04_a'!$D$14</definedName>
-    <definedName name="solver_lhs3" localSheetId="4" hidden="1">'04_b'!$D$14</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'04_a'!$F$11:$F$13</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">'04_b'!$F$11:$F$13</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'03_a'!$B$14</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">'03_b'!$B$14</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">'03_c'!$B$14</definedName>
     <definedName name="solver_lhs4" localSheetId="3" hidden="1">'04_a'!$E$14</definedName>
-    <definedName name="solver_lhs4" localSheetId="4" hidden="1">'04_b'!$E$14</definedName>
+    <definedName name="solver_lhs4" localSheetId="4" hidden="1">'04_b'!$I$11:$L$13</definedName>
     <definedName name="solver_lhs5" localSheetId="1" hidden="1">'03_b'!$B$7</definedName>
     <definedName name="solver_lhs5" localSheetId="2" hidden="1">'03_c'!$B$3:$B$7</definedName>
     <definedName name="solver_lhs5" localSheetId="3" hidden="1">'04_a'!$F$11</definedName>
-    <definedName name="solver_lhs5" localSheetId="4" hidden="1">'04_b'!$F$11</definedName>
+    <definedName name="solver_lhs5" localSheetId="4" hidden="1">'04_b'!$N$11:$Q$13</definedName>
     <definedName name="solver_lhs6" localSheetId="3" hidden="1">'04_a'!$F$12</definedName>
-    <definedName name="solver_lhs6" localSheetId="4" hidden="1">'04_b'!$F$12</definedName>
+    <definedName name="solver_lhs6" localSheetId="4" hidden="1">'04_b'!$E$14</definedName>
     <definedName name="solver_lhs7" localSheetId="3" hidden="1">'04_a'!$F$13</definedName>
-    <definedName name="solver_lhs7" localSheetId="4" hidden="1">'04_b'!$F$13</definedName>
+    <definedName name="solver_lhs7" localSheetId="4" hidden="1">'04_b'!$F$11</definedName>
+    <definedName name="solver_lhs8" localSheetId="4" hidden="1">'04_b'!$F$12</definedName>
+    <definedName name="solver_lhs9" localSheetId="4" hidden="1">'04_b'!$F$13</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
@@ -112,8 +117,8 @@
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">7</definedName>
-    <definedName name="solver_num" localSheetId="4" hidden="1">7</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
@@ -135,13 +140,14 @@
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">4</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">4</definedName>
+    <definedName name="solver_rel10" localSheetId="4" hidden="1">5</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
@@ -151,7 +157,7 @@
     <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_rel4" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="4" hidden="1">5</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_rel5" localSheetId="3" hidden="1">3</definedName>
@@ -160,34 +166,39 @@
     <definedName name="solver_rel6" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel8" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel9" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">'03_a'!$D$11</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'03_b'!$D$11</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">'03_c'!$D$11</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'04_a'!$B$8</definedName>
-    <definedName name="solver_rhs1" localSheetId="4" hidden="1">'04_b'!$B$8</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">"integer"</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">"integer"</definedName>
+    <definedName name="solver_rhs10" localSheetId="4" hidden="1">"binary"</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'03_a'!$D$12</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">'03_b'!$D$12</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">'03_c'!$D$12</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'04_a'!$C$8</definedName>
-    <definedName name="solver_rhs2" localSheetId="4" hidden="1">'04_b'!$C$8</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'04_a'!$B$8:$E$8</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">'04_b'!$B$8:$E$8</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'03_a'!$D$13</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">'03_b'!$D$13</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">'03_c'!$D$13</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'04_a'!$D$8</definedName>
-    <definedName name="solver_rhs3" localSheetId="4" hidden="1">'04_b'!$D$8</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'04_a'!$F$5:$F$7</definedName>
+    <definedName name="solver_rhs3" localSheetId="4" hidden="1">'04_b'!$F$5:$F$7</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">'03_a'!$D$14</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">'03_b'!$D$14</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">'03_c'!$D$14</definedName>
     <definedName name="solver_rhs4" localSheetId="3" hidden="1">'04_a'!$E$8</definedName>
-    <definedName name="solver_rhs4" localSheetId="4" hidden="1">'04_b'!$E$8</definedName>
+    <definedName name="solver_rhs4" localSheetId="4" hidden="1">"binary"</definedName>
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">'03_b'!$D$15</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">"integer"</definedName>
     <definedName name="solver_rhs5" localSheetId="3" hidden="1">'04_a'!$F$5</definedName>
-    <definedName name="solver_rhs5" localSheetId="4" hidden="1">'04_b'!$F$5</definedName>
+    <definedName name="solver_rhs5" localSheetId="4" hidden="1">'04_b'!$B$11:$E$13</definedName>
     <definedName name="solver_rhs6" localSheetId="3" hidden="1">'04_a'!$F$6</definedName>
-    <definedName name="solver_rhs6" localSheetId="4" hidden="1">'04_b'!$F$6</definedName>
+    <definedName name="solver_rhs6" localSheetId="4" hidden="1">'04_b'!$E$8</definedName>
     <definedName name="solver_rhs7" localSheetId="3" hidden="1">'04_a'!$F$7</definedName>
-    <definedName name="solver_rhs7" localSheetId="4" hidden="1">'04_b'!$F$7</definedName>
+    <definedName name="solver_rhs7" localSheetId="4" hidden="1">'04_b'!$F$5</definedName>
+    <definedName name="solver_rhs8" localSheetId="4" hidden="1">'04_b'!$F$6</definedName>
+    <definedName name="solver_rhs9" localSheetId="4" hidden="1">'04_b'!$F$7</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
@@ -236,8 +247,8 @@
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -259,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
   <si>
     <t>Carrots</t>
   </si>
@@ -345,7 +356,19 @@
     <t>Total Fixed Costs</t>
   </si>
   <si>
-    <t>Objective Fixed Costs</t>
+    <t>y_ij * M</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>peanut butter tax</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>y_5</t>
   </si>
 </sst>
 </file>
@@ -786,13 +809,13 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -815,7 +838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -842,7 +865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -869,7 +892,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -896,7 +919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -923,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -950,7 +973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -965,7 +988,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -980,7 +1003,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -995,7 +1018,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1010,7 +1033,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -1018,7 +1041,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <f>SUMPRODUCT(B3:B7, D3:D7)</f>
         <v>2.3177549194991061</v>
@@ -1037,17 +1060,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1C56EF-4B14-D54B-B52B-05B451158C66}">
   <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1070,7 +1094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1124,7 +1148,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1232,7 +1256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1246,8 +1270,11 @@
       <c r="D11" s="3">
         <v>2000</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1262,7 +1289,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1276,8 +1303,14 @@
       <c r="D13" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1291,8 +1324,14 @@
       <c r="D14" s="3">
         <v>250</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1304,7 +1343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -1312,7 +1351,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <f>SUMPRODUCT(B3:B8, D3:D8)</f>
         <v>2.7445945945945951</v>
@@ -1335,13 +1374,13 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1364,7 +1403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1391,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1418,7 +1457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1445,7 +1484,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1472,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1499,7 +1538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1514,7 +1553,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1529,7 +1568,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1544,7 +1583,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1559,7 +1598,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -1567,7 +1606,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <f>SUMPRODUCT(B3:B7, D3:D7)</f>
         <v>2.4299999999999997</v>
@@ -1590,17 +1629,17 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1620,7 +1659,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1640,7 +1679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1660,7 +1699,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1680,7 +1719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1697,7 +1736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1717,7 +1756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1738,7 +1777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1759,7 +1798,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1780,7 +1819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="6">
         <f xml:space="preserve"> SUM(B11:B13)</f>
         <v>10</v>
@@ -1798,13 +1837,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <f>SUMPRODUCT(B5:E7, B11:E13)</f>
         <v>460</v>
@@ -1818,24 +1857,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB1C8C8-2960-4D74-B02D-5741ABED90CB}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="8" max="8" width="14.75" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1855,7 +1894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1875,7 +1914,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1895,7 +1934,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1915,7 +1954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1933,14 +1972,14 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1974,48 +2013,63 @@
       <c r="L10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C11" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D11" s="8">
         <v>0</v>
       </c>
       <c r="E11" s="8">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F11" s="6">
         <f xml:space="preserve"> SUM(B11:E11)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H11" s="7">
         <v>1</v>
       </c>
       <c r="I11" s="4">
-        <f xml:space="preserve"> IF(B11 &gt;0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" ref="J11:L13" si="0" xml:space="preserve"> IF(C11 &gt;0, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f>I11*N16</f>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ref="O11:Q13" si="0">J11*O16</f>
+        <v>0</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L11" s="4">
+      <c r="Q11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2023,44 +2077,56 @@
         <v>0</v>
       </c>
       <c r="C12" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D12" s="8">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E12" s="8">
         <v>0</v>
       </c>
       <c r="F12" s="6">
         <f xml:space="preserve"> SUM(B12:E12)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H12" s="7">
         <v>2</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" ref="I12:I13" si="1" xml:space="preserve"> IF(B12 &gt;0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N12:N13" si="1">I12*N17</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C13" s="8">
         <v>0</v>
@@ -2069,33 +2135,45 @@
         <v>0</v>
       </c>
       <c r="E13" s="8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F13" s="6">
         <f xml:space="preserve"> SUM(B13:E13)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H13" s="7">
         <v>3</v>
       </c>
       <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="4">
+      <c r="P13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="4">
+      <c r="Q13">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2105,46 +2183,47 @@
       </c>
       <c r="C14" s="6">
         <f xml:space="preserve"> SUM(C11:C13)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D14" s="6">
         <f xml:space="preserve"> SUM(D11:D13)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E14" s="6">
         <f xml:space="preserve"> SUM(E11:E13)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="B16" s="5"/>
       <c r="H16" t="s">
         <v>26</v>
       </c>
       <c r="I16" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
-        <f>SUMPRODUCT(B5:E7, B11:E13)</f>
-        <v>460</v>
-      </c>
-      <c r="B17" s="5">
-        <f xml:space="preserve"> A17 + I17</f>
-        <v>1060</v>
-      </c>
+        <f>SUMPRODUCT(B5:E7, B11:E13) + COUNTIF(N11:Q13, "&gt;0")*I16</f>
+        <v>100</v>
+      </c>
+      <c r="B17" s="5"/>
       <c r="H17" t="s">
         <v>27</v>
       </c>
       <c r="I17" s="4">
-        <f xml:space="preserve"> SUM(I11:L13)*100</f>
-        <v>600</v>
+        <f xml:space="preserve"> COUNTIF(N11:Q13, "&gt;0")*I16</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>